<commit_message>
a lot of the functionality is now ready, but outcommented
Reading in the events needs some focus now.
</commit_message>
<xml_diff>
--- a/documentation/BackLog.xlsx
+++ b/documentation/BackLog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alexander\Desktop\DTM\repo\DarkTimesMississippi\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DC558DC-10CB-407C-9890-7164A3F87BB7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03C54444-5F7D-43E6-AD35-EDFFEA839967}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{A7B45295-4886-4A16-A195-10F19CD96452}"/>
   </bookViews>
@@ -309,12 +309,6 @@
     <t>digital dices</t>
   </si>
   <si>
-    <t>As a user, I want to be able to roll two dices in the digital component.</t>
-  </si>
-  <si>
-    <t>As a user, I want to see a 3D animation when I roll the dices.</t>
-  </si>
-  <si>
     <t>gebeurtenissen</t>
   </si>
   <si>
@@ -412,6 +406,12 @@
   </si>
   <si>
     <t>wk0 test</t>
+  </si>
+  <si>
+    <t>As a user, I want to be able to roll two dices in the digital component, because I won't need physical dices if I can.</t>
+  </si>
+  <si>
+    <t>As a user, I want to see a 3D animation when I roll the dices, because the current animation is boring.</t>
   </si>
 </sst>
 </file>
@@ -1009,7 +1009,7 @@
       <c r="B13" s="3"/>
       <c r="C13" s="6"/>
       <c r="F13" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="G13" s="5"/>
       <c r="H13" s="6"/>
@@ -1021,7 +1021,7 @@
       <c r="B14" s="3"/>
       <c r="C14" s="6"/>
       <c r="F14" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="G14" s="4"/>
       <c r="H14" s="3"/>
@@ -1229,7 +1229,7 @@
   <dimension ref="A1:K15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1582,7 +1582,7 @@
   <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1615,13 +1615,13 @@
         <v>85</v>
       </c>
       <c r="H1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="I1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="J1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
@@ -1631,7 +1631,7 @@
       <c r="B2" s="3"/>
       <c r="C2" s="6"/>
       <c r="D2" t="s">
-        <v>91</v>
+        <v>124</v>
       </c>
       <c r="E2" t="s">
         <v>41</v>
@@ -1653,7 +1653,7 @@
       <c r="B3" s="4"/>
       <c r="C3" s="3"/>
       <c r="D3" t="s">
-        <v>92</v>
+        <v>125</v>
       </c>
       <c r="F3">
         <v>16</v>
@@ -1670,12 +1670,12 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="6"/>
       <c r="D4" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="E4" t="s">
         <v>41</v>
@@ -1692,15 +1692,15 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B5" s="3"/>
       <c r="C5" s="4"/>
       <c r="D5" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E5" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="F5">
         <v>1</v>
@@ -1717,15 +1717,15 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B6" s="3"/>
       <c r="C6" s="4"/>
       <c r="D6" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="E6" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="F6">
         <v>8</v>
@@ -1742,12 +1742,12 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B7" s="5"/>
       <c r="C7" s="3"/>
       <c r="D7" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="F7">
         <v>16</v>
@@ -1755,12 +1755,12 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B8" s="3"/>
       <c r="C8" s="6"/>
       <c r="D8" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E8" t="s">
         <v>41</v>
@@ -1771,12 +1771,12 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B9" s="3"/>
       <c r="C9" s="6"/>
       <c r="D9" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E9" t="s">
         <v>41</v>
@@ -1792,7 +1792,7 @@
       <c r="B10" s="3"/>
       <c r="C10" s="4"/>
       <c r="D10" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E10" t="s">
         <v>41</v>
@@ -1803,12 +1803,12 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
       <c r="D11" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E11" t="s">
         <v>76</v>
@@ -1819,15 +1819,15 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B12" s="3"/>
       <c r="C12" s="4"/>
       <c r="D12" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E12" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="F12">
         <v>4</v>
@@ -1835,12 +1835,12 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B13" s="5"/>
       <c r="C13" s="3"/>
       <c r="D13" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="E13" t="s">
         <v>76</v>
@@ -1856,7 +1856,7 @@
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
       <c r="D14" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E14" t="s">
         <v>43</v>
@@ -1872,10 +1872,10 @@
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
       <c r="D15" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E15" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="F15">
         <v>8</v>
@@ -1888,23 +1888,23 @@
       <c r="B16" s="3"/>
       <c r="C16" s="4"/>
       <c r="D16" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E16" t="s">
         <v>49</v>
       </c>
       <c r="F16" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B17" s="3"/>
       <c r="C17" s="4"/>
       <c r="D17" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E17" t="s">
         <v>49</v>
@@ -1915,15 +1915,15 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
       <c r="D18" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="E18" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="F18">
         <v>40</v>

</xml_diff>

<commit_message>
Auto stash before merge of "development" and "origin/development"
</commit_message>
<xml_diff>
--- a/documentation/BackLog.xlsx
+++ b/documentation/BackLog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alexander\Desktop\DTM\repo\DarkTimesMississippi\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{729E5C9A-3F4E-461B-9EE4-1CF682DC2A12}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C0088F8-B502-4AD3-9003-FEBCA8390039}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{A7B45295-4886-4A16-A195-10F19CD96452}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="119">
   <si>
     <t>Fysieke component</t>
   </si>
@@ -340,27 +340,6 @@
   </si>
   <si>
     <t>game control</t>
-  </si>
-  <si>
-    <t>Naam</t>
-  </si>
-  <si>
-    <t>week 0</t>
-  </si>
-  <si>
-    <t>Alexander &amp; Ariano</t>
-  </si>
-  <si>
-    <t>Sebastian &amp; Todd</t>
-  </si>
-  <si>
-    <t>Michael &amp; Sebastian</t>
-  </si>
-  <si>
-    <t>Michael, Sebastian, Todd</t>
-  </si>
-  <si>
-    <t>wk0 test</t>
   </si>
   <si>
     <t>As a user, I want to be able to roll two dices in the digital component, because I won't need physical dices if I can.</t>
@@ -1579,23 +1558,20 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B86C2C0-33C7-4F98-9D8E-2C995B1FAA04}">
-  <dimension ref="A1:J18"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="17.77734375" customWidth="1"/>
-    <col min="4" max="4" width="134.77734375" customWidth="1"/>
-    <col min="5" max="5" width="22.109375" customWidth="1"/>
-    <col min="6" max="6" width="10.44140625" customWidth="1"/>
-    <col min="8" max="8" width="17.109375" customWidth="1"/>
-    <col min="9" max="9" width="9" customWidth="1"/>
+    <col min="3" max="3" width="143.77734375" customWidth="1"/>
+    <col min="4" max="4" width="10.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -1603,329 +1579,213 @@
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>3</v>
+        <v>84</v>
       </c>
       <c r="D1" t="s">
-        <v>84</v>
-      </c>
-      <c r="E1" t="s">
-        <v>44</v>
-      </c>
-      <c r="F1" t="s">
         <v>85</v>
       </c>
-      <c r="H1" t="s">
-        <v>102</v>
-      </c>
-      <c r="I1" t="s">
-        <v>103</v>
-      </c>
-      <c r="J1" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>90</v>
       </c>
       <c r="B2" s="3"/>
-      <c r="C2" s="6"/>
-      <c r="D2" t="s">
-        <v>109</v>
-      </c>
-      <c r="E2" t="s">
-        <v>41</v>
-      </c>
-      <c r="F2">
+      <c r="C2" t="s">
+        <v>102</v>
+      </c>
+      <c r="D2">
         <v>1</v>
       </c>
-      <c r="H2" t="s">
-        <v>41</v>
-      </c>
-      <c r="I2">
-        <v>14.5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>90</v>
       </c>
       <c r="B3" s="4"/>
-      <c r="C3" s="3"/>
-      <c r="D3" t="s">
-        <v>110</v>
-      </c>
-      <c r="F3">
+      <c r="C3" t="s">
+        <v>103</v>
+      </c>
+      <c r="D3">
         <v>16</v>
       </c>
-      <c r="H3" t="s">
-        <v>76</v>
-      </c>
-      <c r="I3">
-        <v>9</v>
-      </c>
-      <c r="J3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>91</v>
       </c>
       <c r="B4" s="3"/>
-      <c r="C4" s="6"/>
-      <c r="D4" t="s">
-        <v>111</v>
-      </c>
-      <c r="E4" t="s">
-        <v>41</v>
-      </c>
-      <c r="F4">
+      <c r="C4" t="s">
+        <v>104</v>
+      </c>
+      <c r="D4">
         <v>4</v>
       </c>
-      <c r="H4" t="s">
-        <v>43</v>
-      </c>
-      <c r="I4">
-        <v>13.5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>91</v>
       </c>
       <c r="B5" s="3"/>
-      <c r="C5" s="4"/>
-      <c r="D5" t="s">
-        <v>112</v>
-      </c>
-      <c r="E5" t="s">
-        <v>104</v>
-      </c>
-      <c r="F5">
+      <c r="C5" t="s">
+        <v>105</v>
+      </c>
+      <c r="D5">
         <v>1</v>
       </c>
-      <c r="H5" t="s">
-        <v>75</v>
-      </c>
-      <c r="I5">
-        <v>7</v>
-      </c>
-      <c r="J5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:4" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>91</v>
       </c>
       <c r="B6" s="3"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="E6" t="s">
-        <v>104</v>
-      </c>
-      <c r="F6">
+      <c r="C6" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="D6">
         <v>8</v>
       </c>
-      <c r="H6" t="s">
-        <v>50</v>
-      </c>
-      <c r="I6">
-        <v>3</v>
-      </c>
-      <c r="J6">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>91</v>
       </c>
       <c r="B7" s="5"/>
-      <c r="C7" s="3"/>
-      <c r="D7" t="s">
-        <v>114</v>
-      </c>
-      <c r="F7">
+      <c r="C7" t="s">
+        <v>107</v>
+      </c>
+      <c r="D7">
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>92</v>
       </c>
       <c r="B8" s="3"/>
-      <c r="C8" s="6"/>
-      <c r="D8" t="s">
-        <v>115</v>
-      </c>
-      <c r="E8" t="s">
-        <v>41</v>
-      </c>
-      <c r="F8">
+      <c r="C8" t="s">
+        <v>108</v>
+      </c>
+      <c r="D8">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>94</v>
       </c>
       <c r="B9" s="3"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="7" t="s">
-        <v>116</v>
-      </c>
-      <c r="E9" t="s">
-        <v>41</v>
-      </c>
-      <c r="F9">
+      <c r="C9" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="D9">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>87</v>
       </c>
       <c r="B10" s="3"/>
-      <c r="C10" s="4"/>
-      <c r="D10" t="s">
-        <v>117</v>
-      </c>
-      <c r="E10" t="s">
-        <v>41</v>
-      </c>
-      <c r="F10">
+      <c r="C10" t="s">
+        <v>110</v>
+      </c>
+      <c r="D10">
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>95</v>
       </c>
       <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="7" t="s">
-        <v>118</v>
-      </c>
-      <c r="E11" t="s">
-        <v>76</v>
-      </c>
-      <c r="F11">
+      <c r="C11" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="D11">
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>101</v>
       </c>
       <c r="B12" s="3"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="E12" t="s">
-        <v>105</v>
-      </c>
-      <c r="F12">
+      <c r="C12" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="D12">
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>96</v>
       </c>
       <c r="B13" s="5"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="7" t="s">
-        <v>120</v>
-      </c>
-      <c r="E13" t="s">
-        <v>76</v>
-      </c>
-      <c r="F13">
+      <c r="C13" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="D13">
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>86</v>
       </c>
       <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="D14" t="s">
-        <v>121</v>
-      </c>
-      <c r="E14" t="s">
-        <v>43</v>
-      </c>
-      <c r="F14">
+      <c r="C14" t="s">
+        <v>114</v>
+      </c>
+      <c r="D14">
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>86</v>
       </c>
       <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="D15" t="s">
-        <v>122</v>
-      </c>
-      <c r="E15" t="s">
-        <v>106</v>
-      </c>
-      <c r="F15">
+      <c r="C15" t="s">
+        <v>115</v>
+      </c>
+      <c r="D15">
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>86</v>
       </c>
       <c r="B16" s="3"/>
-      <c r="C16" s="4"/>
+      <c r="C16" t="s">
+        <v>116</v>
+      </c>
       <c r="D16" t="s">
-        <v>123</v>
-      </c>
-      <c r="E16" t="s">
-        <v>49</v>
-      </c>
-      <c r="F16" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>97</v>
       </c>
       <c r="B17" s="3"/>
-      <c r="C17" s="4"/>
-      <c r="D17" t="s">
-        <v>124</v>
-      </c>
-      <c r="E17" t="s">
-        <v>49</v>
-      </c>
-      <c r="F17">
+      <c r="C17" t="s">
+        <v>117</v>
+      </c>
+      <c r="D17">
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>98</v>
       </c>
       <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
-      <c r="D18" t="s">
-        <v>125</v>
-      </c>
-      <c r="E18" t="s">
-        <v>107</v>
-      </c>
-      <c r="F18">
+      <c r="C18" t="s">
+        <v>118</v>
+      </c>
+      <c r="D18">
         <v>40</v>
       </c>
     </row>

</xml_diff>